<commit_message>
add --new class files
</commit_message>
<xml_diff>
--- a/Python-Basico/relatos.xlsx
+++ b/Python-Basico/relatos.xlsx
@@ -413,14 +413,49 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Producto</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Precio</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Cantidad</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Camisa</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>